<commit_message>
Add convex hull to kml
</commit_message>
<xml_diff>
--- a/locations.xlsx
+++ b/locations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Classes\CSCI585-Database\homeworks\hw3_spatial_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBB7FC39-84D9-4DA4-ABAB-E1513E54FABA}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B3687C73-DDE0-402A-80FE-8C4949649FF5}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20610" windowHeight="14145" xr2:uid="{E412DC9F-C608-4CC0-92EE-17960A3BA5F7}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="179021"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="38">
   <si>
     <t>Young King Restaurant</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -56,10 +57,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Papa's Chicken</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Chase Bank</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -72,14 +69,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>위도</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>경도</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>34; 3; 8</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -136,14 +125,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Lat</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Lng</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>&lt;coordinates&gt;</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -161,6 +142,45 @@
   </si>
   <si>
     <t>Apartment</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Camera Lat</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Camera Lng</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Compass Lat</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Compass Lng</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;name&gt; tag</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;coordinates&gt; tag</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SQL Insert</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>INSERT INTO coordinates(name, lat, lng) VALUES (</t>
+  </si>
+  <si>
+    <t>);</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Papas Chicken</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -534,10 +554,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4738D82-E12E-4C2B-9B09-1C02949011D9}">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7:K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -547,31 +567,41 @@
     <col min="4" max="4" width="12.25" customWidth="1"/>
     <col min="5" max="5" width="12.875" customWidth="1"/>
     <col min="7" max="7" width="36.25" customWidth="1"/>
+    <col min="8" max="8" width="48.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
         <v>10</v>
-      </c>
-      <c r="C1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" t="s">
-        <v>13</v>
       </c>
       <c r="D2" s="1">
         <v>34.052222</v>
@@ -584,19 +614,23 @@
         <v>&lt;name&gt;Apartment&lt;/name&gt;</v>
       </c>
       <c r="H2" t="str">
-        <f>CONCATENATE($H$12,$E2,",",$D2,$H$13)</f>
+        <f t="shared" ref="H2:H10" si="0">CONCATENATE($H$12,$E2,",",$D2,$H$13)</f>
         <v>&lt;coordinates&gt;-118.301944,34.052222&lt;/coordinates&gt;</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I2" t="str">
+        <f>CONCATENATE($I$12, "'", $A2, "', ", $D2, ", ", $E2, $I$13)</f>
+        <v>INSERT INTO coordinates(name, lat, lng) VALUES ('Apartment', 34.052222, -118.301944);</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D3">
         <v>34.052500000000002</v>
@@ -605,23 +639,27 @@
         <v>-118.303056</v>
       </c>
       <c r="G3" t="str">
-        <f t="shared" ref="G3:G10" si="0">CONCATENATE($G$12,$A3,$G$13)</f>
+        <f t="shared" ref="G3:G10" si="1">CONCATENATE($G$12,$A3,$G$13)</f>
         <v>&lt;name&gt;Young King Restaurant&lt;/name&gt;</v>
       </c>
       <c r="H3" t="str">
-        <f>CONCATENATE($H$12,$E3,",",$D3,$H$13)</f>
+        <f t="shared" si="0"/>
         <v>&lt;coordinates&gt;-118.303056,34.0525&lt;/coordinates&gt;</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I3" t="str">
+        <f t="shared" ref="I3:I10" si="2">CONCATENATE($I$12, "'", $A3, "', ", $D3, ", ", $E3, $I$13)</f>
+        <v>INSERT INTO coordinates(name, lat, lng) VALUES ('Young King Restaurant', 34.0525, -118.303056);</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
         <v>14</v>
-      </c>
-      <c r="C4" t="s">
-        <v>17</v>
       </c>
       <c r="D4">
         <v>34.052500000000002</v>
@@ -630,23 +668,27 @@
         <v>-118.30416700000001</v>
       </c>
       <c r="G4" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;name&gt;Yeop Dduk&lt;/name&gt;</v>
+      </c>
+      <c r="H4" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;name&gt;Yeop Dduk&lt;/name&gt;</v>
-      </c>
-      <c r="H4" t="str">
-        <f>CONCATENATE($H$12,$E4,",",$D4,$H$13)</f>
         <v>&lt;coordinates&gt;-118.304167,34.0525&lt;/coordinates&gt;</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I4" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO coordinates(name, lat, lng) VALUES ('Yeop Dduk', 34.0525, -118.304167);</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D5">
         <v>34.053055999999998</v>
@@ -655,23 +697,27 @@
         <v>-118.30374999999999</v>
       </c>
       <c r="G5" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;name&gt;Hite Lounge&lt;/name&gt;</v>
+      </c>
+      <c r="H5" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;name&gt;Hite Lounge&lt;/name&gt;</v>
-      </c>
-      <c r="H5" t="str">
-        <f>CONCATENATE($H$12,$E5,",",$D5,$H$13)</f>
         <v>&lt;coordinates&gt;-118.30375,34.053056&lt;/coordinates&gt;</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I5" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO coordinates(name, lat, lng) VALUES ('Hite Lounge', 34.053056, -118.30375);</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D6">
         <v>34.052778000000004</v>
@@ -680,23 +726,27 @@
         <v>-118.30194400000001</v>
       </c>
       <c r="G6" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;name&gt;Homeshopping World&lt;/name&gt;</v>
+      </c>
+      <c r="H6" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;name&gt;Homeshopping World&lt;/name&gt;</v>
-      </c>
-      <c r="H6" t="str">
-        <f>CONCATENATE($H$12,$E6,",",$D6,$H$13)</f>
         <v>&lt;coordinates&gt;-118.301944,34.052778&lt;/coordinates&gt;</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I6" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO coordinates(name, lat, lng) VALUES ('Homeshopping World', 34.052778, -118.301944);</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D7">
         <v>34.053139000000002</v>
@@ -705,23 +755,27 @@
         <v>-118.30161099999999</v>
       </c>
       <c r="G7" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;name&gt;SleepEZ&lt;/name&gt;</v>
+      </c>
+      <c r="H7" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;name&gt;SleepEZ&lt;/name&gt;</v>
-      </c>
-      <c r="H7" t="str">
-        <f>CONCATENATE($H$12,$E7,",",$D7,$H$13)</f>
         <v>&lt;coordinates&gt;-118.301611,34.053139&lt;/coordinates&gt;</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I7" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO coordinates(name, lat, lng) VALUES ('SleepEZ', 34.053139, -118.301611);</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D8">
         <v>34.052778000000004</v>
@@ -730,23 +784,27 @@
         <v>-118.300556</v>
       </c>
       <c r="G8" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;name&gt;Papas Chicken&lt;/name&gt;</v>
+      </c>
+      <c r="H8" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;name&gt;Papa's Chicken&lt;/name&gt;</v>
-      </c>
-      <c r="H8" t="str">
-        <f>CONCATENATE($H$12,$E8,",",$D8,$H$13)</f>
         <v>&lt;coordinates&gt;-118.300556,34.052778&lt;/coordinates&gt;</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I8" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO coordinates(name, lat, lng) VALUES ('Papas Chicken', 34.052778, -118.300556);</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D9">
         <v>34.052222</v>
@@ -755,23 +813,27 @@
         <v>-118.299722</v>
       </c>
       <c r="G9" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;name&gt;Chase Bank&lt;/name&gt;</v>
+      </c>
+      <c r="H9" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;name&gt;Chase Bank&lt;/name&gt;</v>
-      </c>
-      <c r="H9" t="str">
-        <f>CONCATENATE($H$12,$E9,",",$D9,$H$13)</f>
         <v>&lt;coordinates&gt;-118.299722,34.052222&lt;/coordinates&gt;</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I9" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO coordinates(name, lat, lng) VALUES ('Chase Bank', 34.052222, -118.299722);</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
-        <v>12</v>
-      </c>
       <c r="C10" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D10">
         <v>34.052222</v>
@@ -780,39 +842,49 @@
         <v>-118.300833</v>
       </c>
       <c r="G10" t="str">
+        <f t="shared" si="1"/>
+        <v>&lt;name&gt;Guelaguetza Restaurant&lt;/name&gt;</v>
+      </c>
+      <c r="H10" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;name&gt;Guelaguetza Restaurant&lt;/name&gt;</v>
-      </c>
-      <c r="H10" t="str">
-        <f>CONCATENATE($H$12,$E10,",",$D10,$H$13)</f>
         <v>&lt;coordinates&gt;-118.300833,34.052222&lt;/coordinates&gt;</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I10" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO coordinates(name, lat, lng) VALUES ('Guelaguetza Restaurant', 34.052222, -118.300833);</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G12" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="H12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+      <c r="I12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G13" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="H13" t="s">
-        <v>29</v>
+        <v>24</v>
+      </c>
+      <c r="I13" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B17" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C17" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D17">
         <v>34.051943999999999</v>
@@ -830,10 +902,10 @@
         <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C18" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D18">
         <v>34.052778000000004</v>
@@ -851,10 +923,10 @@
         <v>3</v>
       </c>
       <c r="B19" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C19" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D19">
         <v>34.052778000000004</v>

</xml_diff>